<commit_message>
Saida em csv pronta
</commit_message>
<xml_diff>
--- a/Instancias/teste.xlsx
+++ b/Instancias/teste.xlsx
@@ -300,8 +300,8 @@
   </sheetPr>
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I44" activeCellId="0" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Refatorando e comentando código
</commit_message>
<xml_diff>
--- a/Instancias/teste.xlsx
+++ b/Instancias/teste.xlsx
@@ -58,10 +58,10 @@
     <t xml:space="preserve">d</t>
   </si>
   <si>
-    <t xml:space="preserve">Projeto Integrado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aspectos Humanos em Computação </t>
+    <t xml:space="preserve">Projeto Integrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspectos Humanos em Computação</t>
   </si>
   <si>
     <t xml:space="preserve">Modelagem Computacional</t>
@@ -139,13 +139,13 @@
     <t xml:space="preserve">Metodologia Cientifica</t>
   </si>
   <si>
-    <t xml:space="preserve">Introdução à Administração </t>
+    <t xml:space="preserve">Introdução à Administração</t>
   </si>
   <si>
     <t xml:space="preserve">Gestão e Governança de TI</t>
   </si>
   <si>
-    <t xml:space="preserve">Empreendedorismo e Inovação </t>
+    <t xml:space="preserve">Empreendedorismo e Inovação</t>
   </si>
   <si>
     <t xml:space="preserve">Economia da Informação</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">Comportamento Organizacional I</t>
   </si>
   <si>
-    <t xml:space="preserve">Empreendedorismo Tecnológico </t>
+    <t xml:space="preserve">Empreendedorismo Tecnológico</t>
   </si>
   <si>
     <t xml:space="preserve">Tópicos em ADG</t>
@@ -300,8 +300,8 @@
   </sheetPr>
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I44" activeCellId="0" sqref="I44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>